<commit_message>
Recalibrated transition probabilities. Model now rescales very high adjusted probabilities to maintain sum=1.
</commit_message>
<xml_diff>
--- a/Data/Asthma/Transition probabilities/transition data _ weekly.xlsx
+++ b/Data/Asthma/Transition probabilities/transition data _ weekly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\Climate - Health\Modeling\Data\Asthma\Transition probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8E423E-0E92-4861-902E-437F029CCAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FCB872-5A7D-4680-822E-A60CCF49DD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="-735" windowWidth="21600" windowHeight="12615" tabRatio="697" activeTab="1" xr2:uid="{9B6F3090-D219-4CD1-9FEE-A2B042DB449C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="697" xr2:uid="{9B6F3090-D219-4CD1-9FEE-A2B042DB449C}"/>
   </bookViews>
   <sheets>
     <sheet name="transition_prob" sheetId="1" r:id="rId1"/>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFE29CD-D7CE-45DF-83DF-7AAE57E0BCAE}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1309,10 +1309,10 @@
         <v>2.5319999999999999E-2</v>
       </c>
       <c r="F3" s="33">
-        <v>2.5319999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G3" s="33">
-        <v>5.0099999999999997E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="H3" s="33">
         <v>0</v>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="J3" s="25">
         <f t="shared" ref="J3:J7" si="0">1-SUM(B3:I3)</f>
-        <v>0.68596999999999997</v>
+        <v>0.68979999999999997</v>
       </c>
       <c r="K3" s="35"/>
       <c r="M3" s="8" t="s">
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="33">
-        <v>1.511E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D7" s="33">
         <v>2.5319999999999999E-2</v>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="J7" s="25">
         <f t="shared" si="0"/>
-        <v>0.69162999999999997</v>
+        <v>0.68674000000000002</v>
       </c>
       <c r="K7" s="16"/>
       <c r="M7" s="32" t="s">
@@ -1624,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC26E5-69A8-44D2-8549-2CF52401B436}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3405,7 +3405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C40997-5825-4458-A72C-E6102474C10A}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>